<commit_message>
work with short newTxt
</commit_message>
<xml_diff>
--- a/bin/Debug/net8.0-windows/book.xlsx
+++ b/bin/Debug/net8.0-windows/book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\ExcelTextReplacer\bin\Debug\net8.0-windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kloshar\programming\ExcelTextReplacer\bin\Debug\net8.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0C08BA-45AD-4B5E-86D4-D60ECC4A743E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B6B64B-F3EB-4AC0-BFBE-C2FE56998E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27840" windowHeight="16440" xr2:uid="{EA25952D-A024-4970-BCCD-3DD57D7BA55B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{EA25952D-A024-4970-BCCD-3DD57D7BA55B}"/>
   </bookViews>
   <sheets>
     <sheet name="Плановая2" sheetId="1" r:id="rId1"/>
@@ -34,16 +34,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <x:si>
-    <x:t>xyzz</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>abcd</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,16 +443,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39210354-86BC-476D-BB2E-FACD51380237}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.875" customWidth="1"/>
+    <col min="1" max="1" width="71.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>